<commit_message>
finishing touches for deleiverable 2
</commit_message>
<xml_diff>
--- a/documents/FlyingMongeese_Deliverable_1_ProductBacklog.xlsx
+++ b/documents/FlyingMongeese_Deliverable_1_ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BFF28C-1429-40BB-9EC5-10AB690409D9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3866A0A0-AEA8-4370-AB64-F6E69C1DC96F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12705" yWindow="435" windowWidth="12900" windowHeight="15555" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>W</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>As a small business owner,I want to be able to predict the amount of income on a certain day so that I can account for potential sales</t>
@@ -469,7 +466,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -513,7 +510,7 @@
       <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
         <v>8</v>
       </c>
       <c r="G2" s="2"/>
@@ -523,7 +520,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6">
@@ -532,7 +529,7 @@
       <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
         <v>8</v>
       </c>
       <c r="G3" s="7"/>
@@ -544,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1">
@@ -553,8 +550,8 @@
       <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
+      <c r="F4" s="1">
+        <v>6</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -563,7 +560,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1">
@@ -572,8 +569,8 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
+      <c r="F5" s="1">
+        <v>4</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -582,7 +579,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="1">
@@ -591,8 +588,8 @@
       <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
+      <c r="F6" s="1">
+        <v>4</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -601,10 +598,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -612,8 +609,8 @@
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
+      <c r="F7" s="1">
+        <v>5</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -622,19 +619,19 @@
         <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="1">
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
+      <c r="F8" s="1">
+        <v>2</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -643,10 +640,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1">
         <v>8</v>
@@ -654,8 +651,8 @@
       <c r="E9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
+      <c r="F9" s="1">
+        <v>2</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -664,7 +661,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1">
@@ -673,8 +670,8 @@
       <c r="E10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
+      <c r="F10" s="1">
+        <v>2</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -683,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="1">
@@ -692,8 +689,8 @@
       <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
+      <c r="F11" s="1">
+        <v>6</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -702,10 +699,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>10</v>
@@ -713,13 +710,13 @@
       <c r="E12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>8</v>
+      <c r="F12" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="5"/>
@@ -761,14 +758,14 @@
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="1" t="s">
-        <v>8</v>
+      <c r="F18" s="1">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>